<commit_message>
Improving plots and removed detectCores
</commit_message>
<xml_diff>
--- a/Zetas_Sow_func.xlsx
+++ b/Zetas_Sow_func.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF9D86-F850-4026-8C57-6FE40576DADD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A993DD84-0308-46AB-8B43-A40D0AC74C3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,14 +267,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +558,8 @@
   <dimension ref="A1:XFC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20:H22"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>2.3000000000000001E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="G8" s="8">
         <v>0.12</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>2.3000000000000001E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="G9" s="8">
         <v>0.12</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="8">
-        <v>2.3000000000000001E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="G10" s="8">
         <v>0.12</v>
@@ -1221,10 +1221,10 @@
         <v>5</v>
       </c>
       <c r="E17" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F17" s="14">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G17" s="14">
         <v>0.12</v>
@@ -1262,10 +1262,10 @@
         <v>6</v>
       </c>
       <c r="E18" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F18" s="14">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G18" s="14">
         <v>0.12</v>
@@ -1303,10 +1303,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F19" s="14">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G19" s="14">
         <v>0.12</v>
@@ -1352,7 +1352,7 @@
       <c r="G20" s="16">
         <v>0.15</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H20" s="42">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I20"/>
@@ -1393,7 +1393,7 @@
       <c r="G21" s="16">
         <v>0.15</v>
       </c>
-      <c r="H21" s="45">
+      <c r="H21" s="42">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I21"/>
@@ -1434,7 +1434,7 @@
       <c r="G22" s="16">
         <v>0.15</v>
       </c>
-      <c r="H22" s="45">
+      <c r="H22" s="42">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I22"/>
@@ -1475,7 +1475,7 @@
       <c r="G23" s="18">
         <v>0.12</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="43">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I23"/>
@@ -1516,7 +1516,7 @@
       <c r="G24" s="18">
         <v>0.12</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="43">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I24"/>
@@ -1557,7 +1557,7 @@
       <c r="G25" s="18">
         <v>0.12</v>
       </c>
-      <c r="H25" s="46">
+      <c r="H25" s="43">
         <v>3.4999999999999998E-10</v>
       </c>
       <c r="I25"/>
@@ -1590,10 +1590,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="21">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F26" s="20">
-        <v>5.2999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G26" s="20">
         <v>0.12</v>
@@ -1631,10 +1631,10 @@
         <v>6</v>
       </c>
       <c r="E27" s="21">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F27" s="20">
-        <v>5.2999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G27" s="20">
         <v>0.12</v>
@@ -1672,10 +1672,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="27">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F28" s="26">
-        <v>5.2999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G28" s="26">
         <v>0.12</v>
@@ -1735,8 +1735,8 @@
       <c r="E30" s="5">
         <v>0</v>
       </c>
-      <c r="F30" s="47">
-        <v>9.5000000000000005E-5</v>
+      <c r="F30" s="44">
+        <v>9.1000000000000003E-5</v>
       </c>
       <c r="G30" s="4">
         <v>0.35</v>
@@ -1762,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>9.3999999999999994E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="G31" s="4">
         <v>0.35</v>
@@ -1788,8 +1788,8 @@
         <v>0</v>
       </c>
       <c r="F32" s="6">
-        <f>0.000115</f>
-        <v>1.15E-4</v>
+        <f>0.000135</f>
+        <v>1.35E-4</v>
       </c>
       <c r="G32" s="6">
         <v>0.3</v>
@@ -1815,8 +1815,8 @@
         <v>0</v>
       </c>
       <c r="F33" s="6">
-        <f>0.000112</f>
-        <v>1.12E-4</v>
+        <f>0.000125</f>
+        <v>1.25E-4</v>
       </c>
       <c r="G33" s="6">
         <v>0.3</v>
@@ -1842,8 +1842,8 @@
         <v>0</v>
       </c>
       <c r="F34" s="6">
-        <f>0.000112</f>
-        <v>1.12E-4</v>
+        <f>0.000123</f>
+        <v>1.2300000000000001E-4</v>
       </c>
       <c r="G34" s="6">
         <v>0.3</v>
@@ -1869,8 +1869,8 @@
         <v>0</v>
       </c>
       <c r="F35" s="8">
-        <f>0.00026</f>
-        <v>2.5999999999999998E-4</v>
+        <f>0.00029</f>
+        <v>2.9E-4</v>
       </c>
       <c r="G35" s="8">
         <v>0.25</v>
@@ -1950,7 +1950,7 @@
         <v>0.06</v>
       </c>
       <c r="F38" s="10">
-        <v>5.33E-2</v>
+        <v>5.3400000000000003E-2</v>
       </c>
       <c r="G38" s="10">
         <v>0.3</v>
@@ -1990,7 +1990,7 @@
         <v>0.06</v>
       </c>
       <c r="F39" s="10">
-        <v>5.3100000000000001E-2</v>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="G39" s="10">
         <v>0.3</v>
@@ -2030,7 +2030,7 @@
         <v>0.06</v>
       </c>
       <c r="F40" s="10">
-        <v>5.3600000000000002E-2</v>
+        <v>5.3699999999999998E-2</v>
       </c>
       <c r="G40" s="10">
         <v>0.3</v>
@@ -2070,7 +2070,7 @@
         <v>0.06</v>
       </c>
       <c r="F41" s="12">
-        <v>5.7000000000000002E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G41" s="12">
         <v>0.3</v>
@@ -2109,7 +2109,7 @@
         <v>0.06</v>
       </c>
       <c r="F42" s="12">
-        <v>5.8000000000000003E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="G42" s="12">
         <v>0.3</v>
@@ -2148,7 +2148,7 @@
         <v>0.06</v>
       </c>
       <c r="F43" s="12">
-        <v>5.8000000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="G43" s="12">
         <v>0.3</v>
@@ -2184,10 +2184,10 @@
         <v>5</v>
       </c>
       <c r="E44" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F44" s="14">
-        <v>8.7999999999999995E-2</v>
+        <v>0.09</v>
       </c>
       <c r="G44" s="14">
         <v>0.26</v>
@@ -2223,10 +2223,10 @@
         <v>6</v>
       </c>
       <c r="E45" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F45" s="14">
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G45" s="14">
         <v>0.26</v>
@@ -2262,10 +2262,10 @@
         <v>7</v>
       </c>
       <c r="E46" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F46" s="14">
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G46" s="14">
         <v>0.26</v>
@@ -2304,7 +2304,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F47" s="24">
-        <v>9.5000000000000001E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="G47" s="24">
         <v>0.3</v>
@@ -51468,7 +51468,7 @@
         <v>0.06</v>
       </c>
       <c r="F50" s="18">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="G50" s="18">
         <v>0.3</v>
@@ -51494,7 +51494,7 @@
         <v>0.06</v>
       </c>
       <c r="F51" s="18">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G51" s="18">
         <v>0.3</v>
@@ -51520,7 +51520,7 @@
         <v>0.06</v>
       </c>
       <c r="F52" s="18">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G52" s="18">
         <v>0.3</v>
@@ -51543,7 +51543,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="21">
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F53" s="20">
         <v>0.2</v>
@@ -51551,7 +51551,7 @@
       <c r="G53" s="20">
         <v>0.26</v>
       </c>
-      <c r="H53" s="48">
+      <c r="H53" s="45">
         <v>1.5E-10</v>
       </c>
     </row>
@@ -51569,7 +51569,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="21">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F54" s="20">
         <v>0.18</v>
@@ -51577,7 +51577,7 @@
       <c r="G54" s="20">
         <v>0.26</v>
       </c>
-      <c r="H54" s="48">
+      <c r="H54" s="45">
         <v>1.5E-10</v>
       </c>
     </row>
@@ -51595,7 +51595,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="27">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F55" s="26">
         <v>0.17</v>
@@ -51603,7 +51603,7 @@
       <c r="G55" s="26">
         <v>0.26</v>
       </c>
-      <c r="H55" s="49">
+      <c r="H55" s="46">
         <v>1.5E-10</v>
       </c>
     </row>
@@ -51624,7 +51624,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="8">
-        <v>9.0000000000000006E-5</v>
+        <v>8.7999999999999998E-5</v>
       </c>
       <c r="G56" s="8">
         <v>0.1</v>
@@ -51699,17 +51699,16 @@
         <v>5</v>
       </c>
       <c r="E59" s="11">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F59" s="10">
-        <v>9.7999999999999997E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G59" s="10">
         <v>0.1</v>
       </c>
-      <c r="H59" s="42">
-        <f>0.000000004</f>
-        <v>4.0000000000000002E-9</v>
+      <c r="H59" s="47">
+        <v>3.3999999999999998E-9</v>
       </c>
       <c r="I59"/>
       <c r="J59"/>
@@ -51740,17 +51739,16 @@
         <v>6</v>
       </c>
       <c r="E60" s="11">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F60" s="10">
-        <v>9.7999999999999997E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G60" s="10">
         <v>0.1</v>
       </c>
-      <c r="H60" s="42">
-        <f>0.000000005*0.8</f>
-        <v>4.0000000000000002E-9</v>
+      <c r="H60" s="47">
+        <v>3.3999999999999998E-9</v>
       </c>
       <c r="I60"/>
       <c r="J60"/>
@@ -51781,17 +51779,16 @@
         <v>7</v>
       </c>
       <c r="E61" s="11">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F61" s="10">
-        <v>9.7999999999999997E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G61" s="10">
         <v>0.1</v>
       </c>
-      <c r="H61" s="42">
-        <f>0.000000005*0.8</f>
-        <v>4.0000000000000002E-9</v>
+      <c r="H61" s="47">
+        <v>3.3999999999999998E-9</v>
       </c>
       <c r="I61"/>
       <c r="J61"/>
@@ -51822,16 +51819,16 @@
         <v>5</v>
       </c>
       <c r="E62" s="13">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F62" s="12">
-        <v>9.8999999999999999E-4</v>
+        <v>1.15E-3</v>
       </c>
       <c r="G62" s="12">
         <v>0.1</v>
       </c>
-      <c r="H62" s="43">
-        <v>4.0000000000000002E-9</v>
+      <c r="H62" s="48">
+        <v>3.6E-9</v>
       </c>
       <c r="I62"/>
       <c r="J62"/>
@@ -51862,16 +51859,16 @@
         <v>6</v>
       </c>
       <c r="E63" s="13">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F63" s="12">
-        <v>9.8999999999999999E-4</v>
+        <v>1.15E-3</v>
       </c>
       <c r="G63" s="12">
         <v>0.1</v>
       </c>
-      <c r="H63" s="43">
-        <v>4.0000000000000002E-9</v>
+      <c r="H63" s="48">
+        <v>3.6E-9</v>
       </c>
       <c r="I63"/>
       <c r="J63"/>
@@ -51902,16 +51899,16 @@
         <v>7</v>
       </c>
       <c r="E64" s="13">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F64" s="12">
-        <v>9.8999999999999999E-4</v>
+        <v>1.15E-3</v>
       </c>
       <c r="G64" s="12">
         <v>0.1</v>
       </c>
-      <c r="H64" s="43">
-        <v>4.0000000000000002E-9</v>
+      <c r="H64" s="48">
+        <v>3.6E-9</v>
       </c>
       <c r="I64"/>
       <c r="J64"/>
@@ -51942,17 +51939,16 @@
         <v>5</v>
       </c>
       <c r="E65" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F65" s="14">
-        <f>0.00121*0.9</f>
-        <v>1.0889999999999999E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G65" s="14">
         <v>0.1</v>
       </c>
-      <c r="H65" s="44">
-        <v>4.0000000000000002E-9</v>
+      <c r="H65" s="49">
+        <v>3.6E-9</v>
       </c>
       <c r="I65"/>
       <c r="J65"/>
@@ -51983,17 +51979,16 @@
         <v>6</v>
       </c>
       <c r="E66" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F66" s="14">
-        <f t="shared" ref="F66:F67" si="0">0.00121*0.9</f>
-        <v>1.0889999999999999E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G66" s="14">
         <v>0.1</v>
       </c>
-      <c r="H66" s="44">
-        <v>4.0000000000000002E-9</v>
+      <c r="H66" s="49">
+        <v>3.6E-9</v>
       </c>
       <c r="I66"/>
       <c r="J66"/>
@@ -52024,17 +52019,16 @@
         <v>7</v>
       </c>
       <c r="E67" s="15">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F67" s="14">
-        <f t="shared" si="0"/>
-        <v>1.0889999999999999E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G67" s="14">
         <v>0.1</v>
       </c>
-      <c r="H67" s="44">
-        <v>4.0000000000000002E-9</v>
+      <c r="H67" s="49">
+        <v>3.6E-9</v>
       </c>
       <c r="I67"/>
       <c r="J67"/>
@@ -52065,7 +52059,7 @@
         <v>5</v>
       </c>
       <c r="E68" s="25">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F68" s="24">
         <v>2.2000000000000001E-3</v>
@@ -52073,7 +52067,7 @@
       <c r="G68" s="24">
         <v>0.1</v>
       </c>
-      <c r="H68" s="45">
+      <c r="H68" s="42">
         <f>0.0000000045*0.8</f>
         <v>3.6E-9</v>
       </c>
@@ -52092,7 +52086,7 @@
         <v>6</v>
       </c>
       <c r="E69" s="25">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F69" s="24">
         <v>2.2000000000000001E-3</v>
@@ -52100,8 +52094,8 @@
       <c r="G69" s="24">
         <v>0.1</v>
       </c>
-      <c r="H69" s="45">
-        <f t="shared" ref="H69:H70" si="1">0.0000000045*0.8</f>
+      <c r="H69" s="42">
+        <f t="shared" ref="H69:H70" si="0">0.0000000045*0.8</f>
         <v>3.6E-9</v>
       </c>
     </row>
@@ -52119,7 +52113,7 @@
         <v>7</v>
       </c>
       <c r="E70" s="25">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F70" s="24">
         <v>2.2000000000000001E-3</v>
@@ -52127,8 +52121,8 @@
       <c r="G70" s="24">
         <v>0.1</v>
       </c>
-      <c r="H70" s="45">
-        <f t="shared" si="1"/>
+      <c r="H70" s="42">
+        <f t="shared" si="0"/>
         <v>3.6E-9</v>
       </c>
     </row>
@@ -52146,15 +52140,15 @@
         <v>5</v>
       </c>
       <c r="E71" s="19">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F71" s="18">
-        <v>2.2000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="G71" s="18">
         <v>0.1</v>
       </c>
-      <c r="H71" s="46">
+      <c r="H71" s="43">
         <v>3.6E-9</v>
       </c>
     </row>
@@ -52172,15 +52166,15 @@
         <v>6</v>
       </c>
       <c r="E72" s="19">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F72" s="18">
-        <v>2.2000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="G72" s="18">
         <v>0.1</v>
       </c>
-      <c r="H72" s="46">
+      <c r="H72" s="43">
         <v>3.6E-9</v>
       </c>
     </row>
@@ -52198,15 +52192,15 @@
         <v>7</v>
       </c>
       <c r="E73" s="19">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F73" s="18">
-        <v>2.2000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="G73" s="18">
         <v>0.1</v>
       </c>
-      <c r="H73" s="46">
+      <c r="H73" s="43">
         <v>3.6E-9</v>
       </c>
     </row>
@@ -52224,17 +52218,16 @@
         <v>5</v>
       </c>
       <c r="E74" s="21">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F74" s="20">
-        <f>0.00275*0.9</f>
-        <v>2.4749999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="G74" s="20">
         <v>0.1</v>
       </c>
       <c r="H74" s="20">
-        <v>3.6E-9</v>
+        <v>3.3999999999999998E-9</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
@@ -52251,17 +52244,16 @@
         <v>6</v>
       </c>
       <c r="E75" s="21">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F75" s="20">
-        <f t="shared" ref="F75:F76" si="2">0.00275*0.9</f>
-        <v>2.4749999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="G75" s="20">
         <v>0.1</v>
       </c>
       <c r="H75" s="20">
-        <v>3.6E-9</v>
+        <v>3.3999999999999998E-9</v>
       </c>
     </row>
     <row r="76" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -52278,17 +52270,16 @@
         <v>7</v>
       </c>
       <c r="E76" s="27">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F76" s="26">
-        <f t="shared" si="2"/>
-        <v>2.4749999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="G76" s="26">
         <v>0.1</v>
       </c>
       <c r="H76" s="26">
-        <v>3.6E-9</v>
+        <v>3.3999999999999998E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating plots for ms
</commit_message>
<xml_diff>
--- a/Zetas_Sow_func.xlsx
+++ b/Zetas_Sow_func.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Desktop\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09DEB0C-0281-40B5-AF3D-E1B23B0DBEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6FFE7F-F5A5-49A6-8B09-A3C6AAAAF10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -242,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -297,6 +296,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,8 +594,8 @@
   <dimension ref="A1:XFC82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J58" sqref="J58:J64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1916,9 +1925,15 @@
       <c r="E29" s="3">
         <v>0</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="F29" s="43">
+        <v>9.2E-5</v>
+      </c>
+      <c r="G29" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
       <c r="I29" s="52" t="b">
         <v>0</v>
       </c>
@@ -2019,7 +2034,7 @@
         <f>0.000135</f>
         <v>1.35E-4</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="54">
         <v>0.3</v>
       </c>
       <c r="H32" s="6">
@@ -2055,7 +2070,7 @@
         <f>0.000125</f>
         <v>1.25E-4</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="54">
         <v>0.3</v>
       </c>
       <c r="H33" s="6">
@@ -2091,7 +2106,7 @@
         <f>0.000123</f>
         <v>1.2300000000000001E-4</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="54">
         <v>0.3</v>
       </c>
       <c r="H34" s="6">
@@ -2234,7 +2249,7 @@
       <c r="F38" s="10">
         <v>5.3400000000000003E-2</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="55">
         <v>0.3</v>
       </c>
       <c r="H38" s="10">
@@ -2280,7 +2295,7 @@
       <c r="F39" s="10">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="55">
         <v>0.3</v>
       </c>
       <c r="H39" s="10">
@@ -2326,7 +2341,7 @@
       <c r="F40" s="10">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="55">
         <v>0.3</v>
       </c>
       <c r="H40" s="10">
@@ -2372,7 +2387,7 @@
       <c r="F41" s="12">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="56">
         <v>0.3</v>
       </c>
       <c r="H41" s="12">
@@ -2417,7 +2432,7 @@
       <c r="F42" s="12">
         <v>6.3E-2</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="56">
         <v>0.3</v>
       </c>
       <c r="H42" s="12">
@@ -2462,7 +2477,7 @@
       <c r="F43" s="12">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="56">
         <v>0.3</v>
       </c>
       <c r="H43" s="12">
@@ -2642,7 +2657,7 @@
       <c r="F47" s="24">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="57">
         <v>0.3</v>
       </c>
       <c r="H47" s="16">
@@ -19039,7 +19054,7 @@
       <c r="F48" s="24">
         <v>0.11</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G48" s="57">
         <v>0.3</v>
       </c>
       <c r="H48" s="16">
@@ -35436,7 +35451,7 @@
       <c r="F49" s="24">
         <v>0.109</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="57">
         <v>0.3</v>
       </c>
       <c r="H49" s="16">
@@ -51833,7 +51848,7 @@
       <c r="F50" s="18">
         <v>0.15</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="58">
         <v>0.3</v>
       </c>
       <c r="H50" s="18">
@@ -51868,7 +51883,7 @@
       <c r="F51" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G51" s="18">
+      <c r="G51" s="58">
         <v>0.3</v>
       </c>
       <c r="H51" s="18">
@@ -51903,7 +51918,7 @@
       <c r="F52" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G52" s="18">
+      <c r="G52" s="58">
         <v>0.3</v>
       </c>
       <c r="H52" s="18">
@@ -52043,7 +52058,7 @@
       <c r="F56" s="53">
         <v>7.9099999999999998E-5</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="59">
         <v>0.1</v>
       </c>
       <c r="H56" s="4">
@@ -52076,9 +52091,9 @@
         <v>0</v>
       </c>
       <c r="F57" s="53">
-        <v>7.8999999999999996E-5</v>
-      </c>
-      <c r="G57" s="4">
+        <v>7.8800000000000004E-5</v>
+      </c>
+      <c r="G57" s="59">
         <v>0.1</v>
       </c>
       <c r="H57" s="4">
@@ -52111,9 +52126,9 @@
         <v>0</v>
       </c>
       <c r="F58" s="53">
-        <v>7.8899999999999993E-5</v>
-      </c>
-      <c r="G58" s="4">
+        <v>7.86E-5</v>
+      </c>
+      <c r="G58" s="59">
         <v>0.1</v>
       </c>
       <c r="H58" s="4">
@@ -52148,7 +52163,7 @@
       <c r="F59" s="49">
         <v>8.2999999999999998E-5</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59" s="54">
         <v>0.1</v>
       </c>
       <c r="H59" s="6">
@@ -52183,7 +52198,7 @@
       <c r="F60" s="50">
         <v>8.2000000000000001E-5</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60" s="54">
         <v>0.1</v>
       </c>
       <c r="H60" s="6">
@@ -52218,7 +52233,7 @@
       <c r="F61" s="50">
         <v>8.2000000000000001E-5</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G61" s="54">
         <v>0.1</v>
       </c>
       <c r="H61" s="6">
@@ -52253,7 +52268,7 @@
       <c r="F62" s="8">
         <v>8.7999999999999998E-5</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="60">
         <v>0.1</v>
       </c>
       <c r="H62" s="8">
@@ -52288,7 +52303,7 @@
       <c r="F63" s="8">
         <v>8.7999999999999998E-5</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="60">
         <v>0.1</v>
       </c>
       <c r="H63" s="8">
@@ -52323,7 +52338,7 @@
       <c r="F64" s="8">
         <v>8.7999999999999998E-5</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="60">
         <v>0.1</v>
       </c>
       <c r="H64" s="8">
@@ -52358,7 +52373,7 @@
       <c r="F65" s="10">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="G65" s="10">
+      <c r="G65" s="55">
         <v>0.1</v>
       </c>
       <c r="H65" s="46">
@@ -52404,7 +52419,7 @@
       <c r="F66" s="10">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="G66" s="10">
+      <c r="G66" s="55">
         <v>0.1</v>
       </c>
       <c r="H66" s="46">
@@ -52450,7 +52465,7 @@
       <c r="F67" s="10">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="G67" s="10">
+      <c r="G67" s="55">
         <v>0.1</v>
       </c>
       <c r="H67" s="46">
@@ -52496,7 +52511,7 @@
       <c r="F68" s="12">
         <v>1.15E-3</v>
       </c>
-      <c r="G68" s="12">
+      <c r="G68" s="56">
         <v>0.1</v>
       </c>
       <c r="H68" s="47">
@@ -52542,7 +52557,7 @@
       <c r="F69" s="12">
         <v>1.15E-3</v>
       </c>
-      <c r="G69" s="12">
+      <c r="G69" s="56">
         <v>0.1</v>
       </c>
       <c r="H69" s="47">
@@ -52588,7 +52603,7 @@
       <c r="F70" s="12">
         <v>1.15E-3</v>
       </c>
-      <c r="G70" s="12">
+      <c r="G70" s="56">
         <v>0.1</v>
       </c>
       <c r="H70" s="47">
@@ -52634,7 +52649,7 @@
       <c r="F71" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="61">
         <v>0.1</v>
       </c>
       <c r="H71" s="48">
@@ -52680,7 +52695,7 @@
       <c r="F72" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="G72" s="14">
+      <c r="G72" s="61">
         <v>0.1</v>
       </c>
       <c r="H72" s="48">
@@ -52726,7 +52741,7 @@
       <c r="F73" s="14">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="61">
         <v>0.1</v>
       </c>
       <c r="H73" s="48">
@@ -52772,7 +52787,7 @@
       <c r="F74" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G74" s="24">
+      <c r="G74" s="57">
         <v>0.1</v>
       </c>
       <c r="H74" s="41">
@@ -52808,7 +52823,7 @@
       <c r="F75" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G75" s="24">
+      <c r="G75" s="57">
         <v>0.1</v>
       </c>
       <c r="H75" s="41">
@@ -52844,7 +52859,7 @@
       <c r="F76" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G76" s="24">
+      <c r="G76" s="57">
         <v>0.1</v>
       </c>
       <c r="H76" s="41">
@@ -52880,7 +52895,7 @@
       <c r="F77" s="18">
         <v>2.3E-3</v>
       </c>
-      <c r="G77" s="18">
+      <c r="G77" s="58">
         <v>0.1</v>
       </c>
       <c r="H77" s="42">
@@ -52915,7 +52930,7 @@
       <c r="F78" s="18">
         <v>2.3E-3</v>
       </c>
-      <c r="G78" s="18">
+      <c r="G78" s="58">
         <v>0.1</v>
       </c>
       <c r="H78" s="42">
@@ -52950,7 +52965,7 @@
       <c r="F79" s="18">
         <v>2.3E-3</v>
       </c>
-      <c r="G79" s="18">
+      <c r="G79" s="58">
         <v>0.1</v>
       </c>
       <c r="H79" s="42">
@@ -52985,7 +53000,7 @@
       <c r="F80" s="20">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="G80" s="20">
+      <c r="G80" s="62">
         <v>0.1</v>
       </c>
       <c r="H80" s="20">
@@ -53020,7 +53035,7 @@
       <c r="F81" s="20">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="G81" s="20">
+      <c r="G81" s="62">
         <v>0.1</v>
       </c>
       <c r="H81" s="20">
@@ -53055,7 +53070,7 @@
       <c r="F82" s="26">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="G82" s="26">
+      <c r="G82" s="63">
         <v>0.1</v>
       </c>
       <c r="H82" s="26">

</xml_diff>